<commit_message>
stats de structure #27
</commit_message>
<xml_diff>
--- a/fichiers/conf/modele_statsstructure.xlsx
+++ b/fichiers/conf/modele_statsstructure.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\outilssgdf\fichiers\conf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A2E6E77-6C66-4D84-82E3-E5830A490C37}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C7741CC-E515-42CE-AD15-11FF9B7099B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="1155" windowWidth="25275" windowHeight="13995" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1140" yWindow="1155" windowWidth="21570" windowHeight="11700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chiffres" sheetId="2" r:id="rId1"/>
@@ -418,11 +418,39 @@
     <cellStyle name="Excel Built-in Normal" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="6">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
           <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1044,11 +1072,14 @@
     <mergeCell ref="W4:Y4"/>
   </mergeCells>
   <conditionalFormatting sqref="B5:C1000">
-    <cfRule type="cellIs" dxfId="1" priority="13" operator="lessThan">
+    <cfRule type="cellIs" dxfId="5" priority="14" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="14" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="15" stopIfTrue="1" operator="greaterThanOrEqual">
       <formula>0</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="4" priority="1" stopIfTrue="1">
+      <formula>LEN(TRIM(B5))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
stats de structure #27 : Ajout d'un onglet "à la date de l'extraction"
</commit_message>
<xml_diff>
--- a/fichiers/conf/modele_statsstructure.xlsx
+++ b/fichiers/conf/modele_statsstructure.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\outilssgdf\fichiers\conf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59D9AE01-1E0C-4A9E-963D-FD693A11DE26}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70CAA3C4-CB2E-4402-8B10-067A4F6DF317}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="1155" windowWidth="22380" windowHeight="12900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="600" windowWidth="25080" windowHeight="14100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Chiffres" sheetId="2" r:id="rId1"/>
-    <sheet name="Général" sheetId="3" r:id="rId2"/>
+    <sheet name="Par saison (fin de saison)" sheetId="2" r:id="rId1"/>
+    <sheet name="Par saison (date de génération)" sheetId="4" r:id="rId2"/>
+    <sheet name="Général" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="50">
   <si>
     <t>Structure</t>
   </si>
@@ -181,6 +182,9 @@
   </si>
   <si>
     <t>$[IF(I6&lt;&gt;0,((F6*100)/I6)-100,"")]</t>
+  </si>
+  <si>
+    <t>&lt;jt:forEach items="${effectifs_findannee}" var="effectif"&gt;${effectif.groupe}</t>
   </si>
 </sst>
 </file>
@@ -332,7 +336,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -391,6 +395,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -418,7 +428,28 @@
     <cellStyle name="Excel Built-in Normal" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="6">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -725,7 +756,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AH8"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -752,30 +785,30 @@
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="29"/>
-      <c r="D3" s="24" t="s">
+      <c r="C3" s="31"/>
+      <c r="D3" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24" t="s">
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="24" t="s">
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="K3" s="24"/>
-      <c r="L3" s="24"/>
-      <c r="M3" s="25" t="s">
+      <c r="K3" s="26"/>
+      <c r="L3" s="26"/>
+      <c r="M3" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="N3" s="26"/>
-      <c r="O3" s="27"/>
+      <c r="N3" s="28"/>
+      <c r="O3" s="29"/>
       <c r="Q3" s="11"/>
       <c r="R3" s="11"/>
       <c r="S3" s="11"/>
@@ -841,26 +874,26 @@
       </c>
       <c r="Q4" s="11"/>
       <c r="R4" s="16"/>
-      <c r="S4" s="23"/>
-      <c r="T4" s="23"/>
-      <c r="U4" s="23"/>
-      <c r="V4" s="23"/>
-      <c r="W4" s="23"/>
-      <c r="X4" s="23"/>
-      <c r="Y4" s="23"/>
-      <c r="Z4" s="23"/>
-      <c r="AA4" s="23"/>
-      <c r="AB4" s="23"/>
-      <c r="AC4" s="23"/>
-      <c r="AD4" s="23"/>
-      <c r="AE4" s="23"/>
+      <c r="S4" s="25"/>
+      <c r="T4" s="25"/>
+      <c r="U4" s="25"/>
+      <c r="V4" s="25"/>
+      <c r="W4" s="25"/>
+      <c r="X4" s="25"/>
+      <c r="Y4" s="25"/>
+      <c r="Z4" s="25"/>
+      <c r="AA4" s="25"/>
+      <c r="AB4" s="25"/>
+      <c r="AC4" s="25"/>
+      <c r="AD4" s="25"/>
+      <c r="AE4" s="25"/>
       <c r="AF4" s="11"/>
       <c r="AG4" s="11"/>
       <c r="AH4" s="11"/>
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>13</v>
+        <v>49</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>47</v>
@@ -1051,13 +1084,13 @@
     <mergeCell ref="W4:Y4"/>
   </mergeCells>
   <conditionalFormatting sqref="B5:C1000">
-    <cfRule type="cellIs" dxfId="2" priority="14" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="5" priority="14" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="15" stopIfTrue="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="15" stopIfTrue="1" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="0" priority="1" stopIfTrue="1">
+    <cfRule type="containsBlanks" dxfId="3" priority="1" stopIfTrue="1">
       <formula>LEN(TRIM(B5))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1067,6 +1100,351 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC8BF77C-E92B-4239-A7E9-D77F8E9957A6}">
+  <dimension ref="A1:AH8"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="57.5703125" customWidth="1"/>
+    <col min="2" max="3" width="8.7109375" style="2" customWidth="1"/>
+    <col min="4" max="15" width="8.7109375" customWidth="1"/>
+    <col min="18" max="18" width="28.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:34" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="31"/>
+      <c r="D3" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="K3" s="26"/>
+      <c r="L3" s="26"/>
+      <c r="M3" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="N3" s="28"/>
+      <c r="O3" s="29"/>
+      <c r="Q3" s="11"/>
+      <c r="R3" s="11"/>
+      <c r="S3" s="11"/>
+      <c r="T3" s="11"/>
+      <c r="U3" s="11"/>
+      <c r="V3" s="11"/>
+      <c r="W3" s="11"/>
+      <c r="X3" s="11"/>
+      <c r="Y3" s="11"/>
+      <c r="Z3" s="11"/>
+      <c r="AA3" s="11"/>
+      <c r="AB3" s="11"/>
+      <c r="AC3" s="11"/>
+      <c r="AD3" s="11"/>
+      <c r="AE3" s="11"/>
+      <c r="AF3" s="11"/>
+      <c r="AG3" s="11"/>
+      <c r="AH3" s="11"/>
+    </row>
+    <row r="4" spans="1:34" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="J4" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="K4" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="L4" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="M4" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="N4" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="O4" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q4" s="11"/>
+      <c r="R4" s="23"/>
+      <c r="S4" s="25"/>
+      <c r="T4" s="25"/>
+      <c r="U4" s="25"/>
+      <c r="V4" s="25"/>
+      <c r="W4" s="25"/>
+      <c r="X4" s="25"/>
+      <c r="Y4" s="25"/>
+      <c r="Z4" s="25"/>
+      <c r="AA4" s="25"/>
+      <c r="AB4" s="25"/>
+      <c r="AC4" s="25"/>
+      <c r="AD4" s="25"/>
+      <c r="AE4" s="25"/>
+      <c r="AF4" s="11"/>
+      <c r="AG4" s="11"/>
+      <c r="AH4" s="11"/>
+    </row>
+    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="J5" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="K5" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="L5" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="M5" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="N5" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="O5" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="P5" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q5" s="9"/>
+      <c r="R5" s="23"/>
+      <c r="S5" s="23"/>
+      <c r="T5" s="23"/>
+      <c r="U5" s="23"/>
+      <c r="V5" s="23"/>
+      <c r="W5" s="23"/>
+      <c r="X5" s="23"/>
+      <c r="Y5" s="23"/>
+      <c r="Z5" s="23"/>
+      <c r="AA5" s="23"/>
+      <c r="AB5" s="23"/>
+      <c r="AC5" s="23"/>
+      <c r="AD5" s="23"/>
+      <c r="AE5" s="23"/>
+      <c r="AF5" s="9"/>
+      <c r="AG5" s="9"/>
+      <c r="AH5" s="9"/>
+    </row>
+    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A6" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="H6" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="I6" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="J6" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="K6" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="L6" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="M6" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="N6" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="O6" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="14"/>
+      <c r="S6" s="12"/>
+      <c r="T6" s="12"/>
+      <c r="U6" s="12"/>
+      <c r="V6" s="13"/>
+      <c r="W6" s="12"/>
+      <c r="X6" s="12"/>
+      <c r="Y6" s="13"/>
+      <c r="Z6" s="12"/>
+      <c r="AA6" s="12"/>
+      <c r="AB6" s="13"/>
+      <c r="AC6" s="12"/>
+      <c r="AD6" s="12"/>
+      <c r="AE6" s="13"/>
+      <c r="AF6" s="9"/>
+      <c r="AG6" s="9"/>
+      <c r="AH6" s="9"/>
+    </row>
+    <row r="7" spans="1:34" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="12"/>
+      <c r="N7" s="12"/>
+      <c r="O7" s="13"/>
+      <c r="R7" s="14"/>
+      <c r="S7" s="12"/>
+      <c r="T7" s="12"/>
+      <c r="U7" s="12"/>
+      <c r="V7" s="13"/>
+      <c r="W7" s="12"/>
+      <c r="X7" s="12"/>
+      <c r="Y7" s="13"/>
+      <c r="Z7" s="12"/>
+      <c r="AA7" s="12"/>
+      <c r="AB7" s="13"/>
+      <c r="AC7" s="12"/>
+      <c r="AD7" s="12"/>
+      <c r="AE7" s="13"/>
+    </row>
+    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="Q8" s="9"/>
+      <c r="R8" s="14"/>
+      <c r="S8" s="12"/>
+      <c r="T8" s="12"/>
+      <c r="U8" s="12"/>
+      <c r="V8" s="13"/>
+      <c r="W8" s="12"/>
+      <c r="X8" s="12"/>
+      <c r="Y8" s="13"/>
+      <c r="Z8" s="12"/>
+      <c r="AA8" s="12"/>
+      <c r="AB8" s="13"/>
+      <c r="AC8" s="12"/>
+      <c r="AD8" s="12"/>
+      <c r="AE8" s="13"/>
+      <c r="AF8" s="9"/>
+      <c r="AG8" s="9"/>
+      <c r="AH8" s="9"/>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="W4:Y4"/>
+    <mergeCell ref="Z4:AB4"/>
+    <mergeCell ref="AC4:AE4"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="S4:V4"/>
+  </mergeCells>
+  <conditionalFormatting sqref="B5:C1000">
+    <cfRule type="containsBlanks" dxfId="0" priority="1" stopIfTrue="1">
+      <formula>LEN(TRIM(B5))=0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="2" stopIfTrue="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="3" stopIfTrue="1" operator="greaterThanOrEqual">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC05E892-8D08-47C7-B7DB-21DA32D7D601}">
   <dimension ref="A1:B3"/>
   <sheetViews>

</xml_diff>

<commit_message>
#67 Ajouter l'année 2020 dans la fiche de stats
</commit_message>
<xml_diff>
--- a/fichiers/conf/modele_statsstructure.xlsx
+++ b/fichiers/conf/modele_statsstructure.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\outilssgdf\fichiers\conf\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\analytiscout\fichiers\conf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70CAA3C4-CB2E-4402-8B10-067A4F6DF317}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E223537-260D-49F9-9491-1D9885A76D1C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="600" windowWidth="25080" windowHeight="14100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5190" yWindow="2625" windowWidth="18195" windowHeight="12480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Par saison (fin de saison)" sheetId="2" r:id="rId1"/>
@@ -46,9 +46,6 @@
     <t>2017-2018</t>
   </si>
   <si>
-    <t>2016-2017</t>
-  </si>
-  <si>
     <t>R</t>
   </si>
   <si>
@@ -97,12 +94,6 @@
     <t>${effectif.jeunes.2017}</t>
   </si>
   <si>
-    <t>${effectif.responsables.2016}</t>
-  </si>
-  <si>
-    <t>${effectif.jeunes.2016}</t>
-  </si>
-  <si>
     <t>$[D5+E5]</t>
   </si>
   <si>
@@ -151,9 +142,6 @@
     <t>$[SUM(O5)]</t>
   </si>
   <si>
-    <t>2019-2020</t>
-  </si>
-  <si>
     <t>Version du modèle</t>
   </si>
   <si>
@@ -185,6 +173,18 @@
   </si>
   <si>
     <t>&lt;jt:forEach items="${effectifs_findannee}" var="effectif"&gt;${effectif.groupe}</t>
+  </si>
+  <si>
+    <t>2020-2019</t>
+  </si>
+  <si>
+    <t>2019-2018</t>
+  </si>
+  <si>
+    <t>${effectif.responsables.2020}</t>
+  </si>
+  <si>
+    <t>${effectif.jeunes.2020}</t>
   </si>
 </sst>
 </file>
@@ -432,13 +432,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="9"/>
         </patternFill>
       </fill>
@@ -447,6 +440,13 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -756,9 +756,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AH8"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -770,7 +768,7 @@
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -778,7 +776,7 @@
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:34" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -786,26 +784,26 @@
         <v>0</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3" s="31"/>
       <c r="D3" s="26" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="E3" s="26"/>
       <c r="F3" s="26"/>
       <c r="G3" s="26" t="s">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="H3" s="26"/>
       <c r="I3" s="26"/>
       <c r="J3" s="26" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K3" s="26"/>
       <c r="L3" s="26"/>
       <c r="M3" s="27" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N3" s="28"/>
       <c r="O3" s="29"/>
@@ -831,46 +829,46 @@
     <row r="4" spans="1:34" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>9</v>
-      </c>
       <c r="D4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="F4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="6" t="s">
-        <v>6</v>
-      </c>
       <c r="G4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="I4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="6" t="s">
-        <v>6</v>
-      </c>
       <c r="J4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="K4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="K4" s="6" t="s">
+      <c r="L4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="L4" s="6" t="s">
-        <v>6</v>
-      </c>
       <c r="M4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="N4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="N4" s="6" t="s">
+      <c r="O4" s="6" t="s">
         <v>5</v>
-      </c>
-      <c r="O4" s="6" t="s">
-        <v>6</v>
       </c>
       <c r="Q4" s="11"/>
       <c r="R4" s="16"/>
@@ -893,52 +891,52 @@
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="B5" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="D5" s="19" t="s">
+      <c r="F5" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="J5" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="20" t="s">
+      <c r="K5" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="L5" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="M5" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="N5" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="O5" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="G5" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="I5" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="J5" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="K5" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="L5" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="M5" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="N5" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="O5" s="20" t="s">
-        <v>25</v>
-      </c>
       <c r="P5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="Q5" s="9"/>
       <c r="R5" s="16"/>
@@ -961,49 +959,49 @@
     </row>
     <row r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D6" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="19" t="s">
+      <c r="G6" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="19" t="s">
+      <c r="I6" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="J6" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="G6" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="H6" s="19" t="s">
+      <c r="K6" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="I6" s="19" t="s">
+      <c r="L6" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="J6" s="19" t="s">
+      <c r="M6" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="K6" s="19" t="s">
+      <c r="N6" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="L6" s="19" t="s">
+      <c r="O6" s="19" t="s">
         <v>34</v>
-      </c>
-      <c r="M6" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="N6" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="O6" s="19" t="s">
-        <v>37</v>
       </c>
       <c r="Q6" s="9"/>
       <c r="R6" s="14"/>
@@ -1115,7 +1113,7 @@
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -1123,7 +1121,7 @@
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:34" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -1131,26 +1129,26 @@
         <v>0</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3" s="31"/>
       <c r="D3" s="26" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="E3" s="26"/>
       <c r="F3" s="26"/>
       <c r="G3" s="26" t="s">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="H3" s="26"/>
       <c r="I3" s="26"/>
       <c r="J3" s="26" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K3" s="26"/>
       <c r="L3" s="26"/>
       <c r="M3" s="27" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N3" s="28"/>
       <c r="O3" s="29"/>
@@ -1176,46 +1174,46 @@
     <row r="4" spans="1:34" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>9</v>
-      </c>
       <c r="D4" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="24" t="s">
+      <c r="F4" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="24" t="s">
-        <v>6</v>
-      </c>
       <c r="G4" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="24" t="s">
+      <c r="I4" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="24" t="s">
-        <v>6</v>
-      </c>
       <c r="J4" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="K4" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="K4" s="24" t="s">
+      <c r="L4" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="L4" s="24" t="s">
-        <v>6</v>
-      </c>
       <c r="M4" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="N4" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="N4" s="24" t="s">
+      <c r="O4" s="24" t="s">
         <v>5</v>
-      </c>
-      <c r="O4" s="24" t="s">
-        <v>6</v>
       </c>
       <c r="Q4" s="11"/>
       <c r="R4" s="23"/>
@@ -1238,52 +1236,52 @@
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="F5" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="D5" s="19" t="s">
+      <c r="I5" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="J5" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="20" t="s">
+      <c r="K5" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="L5" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="M5" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="N5" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="O5" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="G5" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="I5" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="J5" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="K5" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="L5" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="M5" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="N5" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="O5" s="20" t="s">
-        <v>25</v>
-      </c>
       <c r="P5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="Q5" s="9"/>
       <c r="R5" s="23"/>
@@ -1306,49 +1304,49 @@
     </row>
     <row r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D6" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="19" t="s">
+      <c r="G6" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="19" t="s">
+      <c r="I6" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="J6" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="G6" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="H6" s="19" t="s">
+      <c r="K6" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="I6" s="19" t="s">
+      <c r="L6" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="J6" s="19" t="s">
+      <c r="M6" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="K6" s="19" t="s">
+      <c r="N6" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="L6" s="19" t="s">
+      <c r="O6" s="19" t="s">
         <v>34</v>
-      </c>
-      <c r="M6" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="N6" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="O6" s="19" t="s">
-        <v>37</v>
       </c>
       <c r="Q6" s="9"/>
       <c r="R6" s="14"/>
@@ -1429,13 +1427,13 @@
     <mergeCell ref="S4:V4"/>
   </mergeCells>
   <conditionalFormatting sqref="B5:C1000">
-    <cfRule type="containsBlanks" dxfId="0" priority="1" stopIfTrue="1">
+    <cfRule type="containsBlanks" dxfId="2" priority="1" stopIfTrue="1">
       <formula>LEN(TRIM(B5))=0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="2" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="3" stopIfTrue="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="0" priority="3" stopIfTrue="1" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1448,9 +1446,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC05E892-8D08-47C7-B7DB-21DA32D7D601}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1460,26 +1456,26 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B1" s="22">
-        <v>43791</v>
+        <v>44080</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>